<commit_message>
Added slides to Notes.pptx
</commit_message>
<xml_diff>
--- a/output/50x50x5_compare_w_exp/Weibull_constants_diagonals_5.xlsx
+++ b/output/50x50x5_compare_w_exp/Weibull_constants_diagonals_5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtan15\Documents\GitHub\Monte-Carlos-MgO-TDDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtan15\Documents\GitHub\Monte-Carlos-MgO-TDDB\output\50x50x5_compare_w_exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1EB86C-26E2-41AF-8099-5F5F85228C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A916E5BD-F962-49CC-B020-3B2FF21542D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3038,8 +3038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3284,6 +3284,10 @@
       <c r="D11">
         <v>1.0434042992122619E-2</v>
       </c>
+      <c r="E11">
+        <f>AVERAGE(D2:D11)</f>
+        <v>0.67422587202659012</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13">
@@ -3294,6 +3298,10 @@
       </c>
       <c r="D13">
         <v>1.3769469999999999E-3</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(D13:D22)</f>
+        <v>9.9725932000000003E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>